<commit_message>
Fruits of a long day of PAD analysis
Fruits of a long day of PAD analysis with environmental context and
field line tracing
</commit_message>
<xml_diff>
--- a/Ionospheric Outflow/PAD_cases.xlsx
+++ b/Ionospheric Outflow/PAD_cases.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -435,6 +435,14 @@
     <xf numFmtId="164" fontId="0" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -459,14 +467,6 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -774,9 +774,9 @@
   </sheetPr>
   <dimension ref="A1:P48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A6" sqref="A6:XFD6"/>
+      <selection pane="bottomLeft" activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -796,13 +796,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16">
-      <c r="A1" s="44" t="s">
+      <c r="A1" s="48" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="44" t="s">
+      <c r="B1" s="48" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="46" t="s">
+      <c r="C1" s="50" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="22" t="s">
@@ -833,28 +833,28 @@
       <c r="M1" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="N1" s="44" t="s">
+      <c r="N1" s="48" t="s">
         <v>9</v>
       </c>
-      <c r="O1" s="44"/>
-      <c r="P1" s="42" t="s">
+      <c r="O1" s="48"/>
+      <c r="P1" s="46" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:16">
-      <c r="A2" s="44"/>
-      <c r="B2" s="44"/>
-      <c r="C2" s="46"/>
-      <c r="D2" s="47" t="s">
+      <c r="A2" s="48"/>
+      <c r="B2" s="48"/>
+      <c r="C2" s="50"/>
+      <c r="D2" s="51" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="48"/>
-      <c r="F2" s="49"/>
-      <c r="G2" s="43" t="s">
+      <c r="E2" s="52"/>
+      <c r="F2" s="53"/>
+      <c r="G2" s="47" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="44"/>
-      <c r="I2" s="45"/>
+      <c r="H2" s="48"/>
+      <c r="I2" s="49"/>
       <c r="J2" s="20" t="s">
         <v>17</v>
       </c>
@@ -871,7 +871,7 @@
       <c r="O2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="P2" s="42"/>
+      <c r="P2" s="46"/>
     </row>
     <row r="3" spans="1:16">
       <c r="A3" s="6">
@@ -1964,10 +1964,10 @@
       </c>
     </row>
     <row r="34" spans="1:12">
-      <c r="A34" s="50" t="s">
+      <c r="A34" s="42" t="s">
         <v>21</v>
       </c>
-      <c r="B34" s="50">
+      <c r="B34" s="42">
         <v>1</v>
       </c>
     </row>
@@ -1975,44 +1975,44 @@
       <c r="A35" t="s">
         <v>20</v>
       </c>
-      <c r="B35" s="52" t="s">
+      <c r="B35" s="45" t="s">
         <v>22</v>
       </c>
-      <c r="C35" s="52"/>
+      <c r="C35" s="45"/>
     </row>
     <row r="36" spans="1:12" ht="45">
-      <c r="A36" s="51" t="s">
+      <c r="A36" s="43" t="s">
         <v>23</v>
       </c>
-      <c r="B36" s="52"/>
-      <c r="C36" s="52"/>
+      <c r="B36" s="45"/>
+      <c r="C36" s="45"/>
     </row>
     <row r="37" spans="1:12">
       <c r="A37" t="s">
         <v>24</v>
       </c>
-      <c r="B37" s="52"/>
-      <c r="C37" s="52"/>
+      <c r="B37" s="45"/>
+      <c r="C37" s="45"/>
     </row>
     <row r="38" spans="1:12">
       <c r="A38" t="s">
         <v>25</v>
       </c>
-      <c r="B38" s="52"/>
-      <c r="C38" s="52"/>
+      <c r="B38" s="45"/>
+      <c r="C38" s="45"/>
     </row>
     <row r="39" spans="1:12">
       <c r="A39" t="s">
         <v>26</v>
       </c>
-      <c r="B39" s="52"/>
-      <c r="C39" s="52"/>
+      <c r="B39" s="45"/>
+      <c r="C39" s="45"/>
     </row>
     <row r="43" spans="1:12">
-      <c r="A43" s="53" t="s">
+      <c r="A43" s="44" t="s">
         <v>21</v>
       </c>
-      <c r="B43" s="53">
+      <c r="B43" s="44">
         <v>2</v>
       </c>
     </row>
@@ -2020,19 +2020,19 @@
       <c r="A44" t="s">
         <v>20</v>
       </c>
-      <c r="B44" s="52" t="s">
+      <c r="B44" s="45" t="s">
         <v>27</v>
       </c>
-      <c r="C44" s="52"/>
+      <c r="C44" s="45"/>
     </row>
     <row r="45" spans="1:12" ht="45">
-      <c r="A45" s="51" t="s">
+      <c r="A45" s="43" t="s">
         <v>23</v>
       </c>
-      <c r="B45" s="52">
+      <c r="B45" s="45">
         <v>1.43</v>
       </c>
-      <c r="C45" s="52"/>
+      <c r="C45" s="45"/>
       <c r="D45" s="5" t="s">
         <v>28</v>
       </c>
@@ -2042,10 +2042,10 @@
       <c r="A46" t="s">
         <v>24</v>
       </c>
-      <c r="B46" s="52">
+      <c r="B46" s="45">
         <v>5</v>
       </c>
-      <c r="C46" s="52"/>
+      <c r="C46" s="45"/>
       <c r="D46" s="5" t="s">
         <v>29</v>
       </c>
@@ -2055,10 +2055,10 @@
       <c r="A47" t="s">
         <v>25</v>
       </c>
-      <c r="B47" s="52">
+      <c r="B47" s="45">
         <v>-0.4</v>
       </c>
-      <c r="C47" s="52"/>
+      <c r="C47" s="45"/>
       <c r="D47" s="5" t="s">
         <v>29</v>
       </c>
@@ -2068,26 +2068,16 @@
       <c r="A48" t="s">
         <v>26</v>
       </c>
-      <c r="B48" s="52">
+      <c r="B48" s="45">
         <v>4.2</v>
       </c>
-      <c r="C48" s="52"/>
+      <c r="C48" s="45"/>
       <c r="D48" s="5" t="s">
         <v>29</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="B45:C45"/>
-    <mergeCell ref="B46:C46"/>
-    <mergeCell ref="B47:C47"/>
-    <mergeCell ref="B48:C48"/>
-    <mergeCell ref="B35:C35"/>
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="B38:C38"/>
-    <mergeCell ref="B39:C39"/>
     <mergeCell ref="P1:P2"/>
     <mergeCell ref="G2:I2"/>
     <mergeCell ref="A1:A2"/>
@@ -2095,6 +2085,16 @@
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="D2:F2"/>
     <mergeCell ref="N1:O1"/>
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="B46:C46"/>
+    <mergeCell ref="B47:C47"/>
+    <mergeCell ref="B48:C48"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="79" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -2103,12 +2103,28 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1">
+        <f>16/9</f>
+        <v>1.7777777777777777</v>
+      </c>
+      <c r="B1">
+        <v>4</v>
+      </c>
+      <c r="C1">
+        <f>B1*A1</f>
+        <v>7.1111111111111107</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>